<commit_message>
Update To use for equations - surveyFactorsAll_Tracey with SSB data.xlsx
</commit_message>
<xml_diff>
--- a/Tracey's Folder/To use for equations - surveyFactorsAll_Tracey with SSB data.xlsx
+++ b/Tracey's Folder/To use for equations - surveyFactorsAll_Tracey with SSB data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herri\Documents\GitHub\HerringScience.github.io\Tracey's Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DC08F8-ACB1-4C1F-A1A6-4436D1DC3EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9009C9AB-54F7-4340-8E31-6496315E6504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -777,7 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -859,9 +859,6 @@
     </xf>
     <xf numFmtId="22" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1221,34 +1218,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2:X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="8" customWidth="1"/>
-    <col min="4" max="5" width="12.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="0.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="1.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="0.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="15" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="1.140625" customWidth="1"/>
+    <col min="10" max="10" width="0.85546875" customWidth="1"/>
+    <col min="11" max="11" width="0.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.5703125" style="8" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" style="4" customWidth="1"/>
     <col min="16" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.140625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="15" style="2" customWidth="1"/>
-    <col min="21" max="21" width="12" style="2" customWidth="1"/>
-    <col min="22" max="24" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="0.5703125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="1" style="2" customWidth="1"/>
+    <col min="22" max="22" width="1.28515625" customWidth="1"/>
+    <col min="23" max="24" width="17" customWidth="1"/>
     <col min="25" max="25" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1576,7 +1575,7 @@
       <c r="X5" s="11"/>
       <c r="Y5" s="29"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1620,7 +1619,7 @@
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>36413.821527777778</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -22725,7 +22724,7 @@
         <f t="shared" si="70"/>
         <v>-1.033333333209157</v>
       </c>
-      <c r="T262" s="39">
+      <c r="T262" s="2">
         <v>801</v>
       </c>
       <c r="U262" s="2" t="s">
@@ -25869,6 +25868,7 @@
       <c r="AO296" s="22"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AO296" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO296">
     <sortCondition ref="B2:B296"/>
   </sortState>
@@ -25877,12 +25877,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa15ca5b-4450-4fec-8212-75ae51eef6c9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9b77705d-b477-4602-ae15-a5316c12e631" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26081,20 +26083,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa15ca5b-4450-4fec-8212-75ae51eef6c9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9b77705d-b477-4602-ae15-a5316c12e631" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEA89319-F00C-40E2-B422-E7B15BEFCE0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C11BA438-8776-4F92-AF90-A30F82347EBE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa15ca5b-4450-4fec-8212-75ae51eef6c9"/>
+    <ds:schemaRef ds:uri="9b77705d-b477-4602-ae15-a5316c12e631"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26119,12 +26122,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C11BA438-8776-4F92-AF90-A30F82347EBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEA89319-F00C-40E2-B422-E7B15BEFCE0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aa15ca5b-4450-4fec-8212-75ae51eef6c9"/>
-    <ds:schemaRef ds:uri="9b77705d-b477-4602-ae15-a5316c12e631"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>